<commit_message>
the randomizer is working AND going through all the pics available
</commit_message>
<xml_diff>
--- a/FeaturedArtHtmls/Art Database.xlsx
+++ b/FeaturedArtHtmls/Art Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Despi\CodingStuff\MFS-s2-countdown\FeaturedArtHtmls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECA30DB-CA51-4A70-A7DB-408D68118E6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42977C93-F990-4932-AC7F-F22C27E3EFA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{2EBAAF9A-B1F9-487C-9668-FCA382094CB7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="104">
   <si>
     <t>Art_001</t>
   </si>
@@ -322,6 +322,30 @@
   </si>
   <si>
     <t>brunamz</t>
+  </si>
+  <si>
+    <t>https://puddingmv.tumblr.com/post/643034001960009728/she-knelt-to-the-ground-and-pulled-out-a-ring-and</t>
+  </si>
+  <si>
+    <t>puddingmv</t>
+  </si>
+  <si>
+    <t>https://scavenger-rey.tumblr.com/post/643016761353125888/stargazing-date</t>
+  </si>
+  <si>
+    <t>scavenger-rey</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/p/B_29Awenjv3/</t>
+  </si>
+  <si>
+    <t>_camille_pelletier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camille </t>
+  </si>
+  <si>
+    <t>https://brunamz.tumblr.com/post/642424831199051776</t>
   </si>
 </sst>
 </file>
@@ -684,7 +708,7 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1085,25 +1109,52 @@
       <c r="A24" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="B24" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="B25" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
+      <c r="B26" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
@@ -1126,9 +1177,18 @@
       <c r="A28" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
+      <c r="B28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">

</xml_diff>

<commit_message>
added more art, up to 30 now
</commit_message>
<xml_diff>
--- a/FeaturedArtHtmls/Art Database.xlsx
+++ b/FeaturedArtHtmls/Art Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Despi\CodingStuff\MFS-s2-countdown\FeaturedArtHtmls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42977C93-F990-4932-AC7F-F22C27E3EFA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F44D816-4AC2-46F7-AAC7-86E6B672D42C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{2EBAAF9A-B1F9-487C-9668-FCA382094CB7}"/>
+    <workbookView xWindow="0" yWindow="288" windowWidth="23040" windowHeight="12072" xr2:uid="{2EBAAF9A-B1F9-487C-9668-FCA382094CB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="113">
   <si>
     <t>Art_001</t>
   </si>
@@ -346,6 +346,33 @@
   </si>
   <si>
     <t>https://brunamz.tumblr.com/post/642424831199051776</t>
+  </si>
+  <si>
+    <t>https://archiveofourown.org/works/24329308</t>
+  </si>
+  <si>
+    <t>Cap</t>
+  </si>
+  <si>
+    <t>thecaptainspeaks</t>
+  </si>
+  <si>
+    <t>AO3</t>
+  </si>
+  <si>
+    <t>https://archiveofourown.org/users/majesdane</t>
+  </si>
+  <si>
+    <t>Maple</t>
+  </si>
+  <si>
+    <t>majesdane</t>
+  </si>
+  <si>
+    <t>isailonships</t>
+  </si>
+  <si>
+    <t>https://archiveofourown.org/users/ISailOnShips/pseuds/ISailOnShips</t>
   </si>
 </sst>
 </file>
@@ -707,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D4BCFE8-83E7-41BE-B913-61419F14B40F}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1194,25 +1221,52 @@
       <c r="A29" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
+      <c r="B29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
+      <c r="B30" t="s">
+        <v>108</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
+      <c r="B31" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">

</xml_diff>

<commit_message>
submissions added up to response #14
</commit_message>
<xml_diff>
--- a/FeaturedArtHtmls/Art Database.xlsx
+++ b/FeaturedArtHtmls/Art Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Despi\CodingStuff\MFS-s2-countdown\FeaturedArtHtmls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B22138-AC20-4CC4-9AB1-284A0869860C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704E8580-1DA9-4243-B5E5-C5A9C5B93D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="288" windowWidth="23040" windowHeight="12072" xr2:uid="{2EBAAF9A-B1F9-487C-9668-FCA382094CB7}"/>
+    <workbookView xWindow="-972" yWindow="1344" windowWidth="23040" windowHeight="12072" xr2:uid="{2EBAAF9A-B1F9-487C-9668-FCA382094CB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="152">
   <si>
     <t>Art_001</t>
   </si>
@@ -382,6 +382,114 @@
   </si>
   <si>
     <t>https://www.instagram.com/p/CAD6kQFg1ho/?utm_medium=share_sheet</t>
+  </si>
+  <si>
+    <t>https://www.archiveofourown.org/users/blondedreamboy/pseuds/blondedreamboy</t>
+  </si>
+  <si>
+    <t>blondedreamboy</t>
+  </si>
+  <si>
+    <t>To be notified at</t>
+  </si>
+  <si>
+    <t>@blondedreamboy</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/p/CAOa5ggAdBD/?utm_source=ig_web_copy_link</t>
+  </si>
+  <si>
+    <t>Steph</t>
+  </si>
+  <si>
+    <t>callmestephlee</t>
+  </si>
+  <si>
+    <t>Notified? (Y/N)</t>
+  </si>
+  <si>
+    <t>theycallmestephlee</t>
+  </si>
+  <si>
+    <t>https://twitter.com/jmj1812/status/1271541462891724801?s=21</t>
+  </si>
+  <si>
+    <t>Janina</t>
+  </si>
+  <si>
+    <t>Jmj1812</t>
+  </si>
+  <si>
+    <t>https://twitter.com/aymmgreen/status/1364463600862068737</t>
+  </si>
+  <si>
+    <t>Shan Bellweather</t>
+  </si>
+  <si>
+    <t>aymmgreen</t>
+  </si>
+  <si>
+    <t>https://twitter.com/aymmgreen/status/1349658328092217345</t>
+  </si>
+  <si>
+    <t>https://twitter.com/jadededit21/status/1373586371210842115</t>
+  </si>
+  <si>
+    <t>jadededit21</t>
+  </si>
+  <si>
+    <t>https://twitter.com/jadededit21/status/1380147126630498308/photo/1</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/p/CPaqAl8hUD0/</t>
+  </si>
+  <si>
+    <t>Martyphlox</t>
+  </si>
+  <si>
+    <t>I guess same</t>
+  </si>
+  <si>
+    <t>"Twitter or Instagram"</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/p/CPasaDZB_er/</t>
+  </si>
+  <si>
+    <t>https://archiveofourown.org/users/theycallmestephlee/pseuds/theycallmestephlee</t>
+  </si>
+  <si>
+    <t>Art_043</t>
+  </si>
+  <si>
+    <t>Art_044</t>
+  </si>
+  <si>
+    <t>Art_045</t>
+  </si>
+  <si>
+    <t>Art_046</t>
+  </si>
+  <si>
+    <t>Art_047</t>
+  </si>
+  <si>
+    <t>Art_048</t>
+  </si>
+  <si>
+    <t>Art_049</t>
+  </si>
+  <si>
+    <t>Art_050</t>
+  </si>
+  <si>
+    <t>Art_051</t>
+  </si>
+  <si>
+    <t>Art_052</t>
+  </si>
+  <si>
+    <t>Art_053</t>
   </si>
 </sst>
 </file>
@@ -411,7 +519,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -419,14 +527,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -741,18 +888,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D4BCFE8-83E7-41BE-B913-61419F14B40F}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" t="s">
         <v>14</v>
@@ -766,8 +914,15 @@
       <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" s="5"/>
+      <c r="H1" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -784,7 +939,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -801,7 +956,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -818,7 +973,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -835,7 +990,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -852,7 +1007,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -869,7 +1024,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -886,7 +1041,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -903,7 +1058,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -920,7 +1075,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -937,7 +1092,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -954,7 +1109,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -971,7 +1126,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -988,7 +1143,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1005,7 +1160,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>56</v>
       </c>
@@ -1294,7 +1449,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>73</v>
       </c>
@@ -1311,87 +1466,295 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B34" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B35" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>125</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>128</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>131</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>134</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>135</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>139</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
+      <c r="B43" t="s">
+        <v>140</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>151</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>